<commit_message>
Update arch excel and diagram file
</commit_message>
<xml_diff>
--- a/doc/Arch_Beta_Week2.xlsx
+++ b/doc/Arch_Beta_Week2.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="838" uniqueCount="386">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="921" uniqueCount="400">
   <si>
     <t xml:space="preserve">指令</t>
   </si>
@@ -3651,6 +3651,9 @@
     </r>
   </si>
   <si>
+    <t xml:space="preserve">CT.stall</t>
+  </si>
+  <si>
     <t xml:space="preserve">R.rdata1</t>
   </si>
   <si>
@@ -3666,25 +3669,64 @@
     <t xml:space="preserve">E.ex_wdata</t>
   </si>
   <si>
+    <t xml:space="preserve">HI.hi_o</t>
+  </si>
+  <si>
     <t xml:space="preserve">M.wreg_o</t>
   </si>
   <si>
+    <t xml:space="preserve">HI.lo_o</t>
+  </si>
+  <si>
     <t xml:space="preserve">M.wd_o</t>
   </si>
   <si>
+    <t xml:space="preserve">W.hi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C.stall</t>
+  </si>
+  <si>
     <t xml:space="preserve">M.wdata_o</t>
   </si>
   <si>
+    <t xml:space="preserve">W.whilo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">M.hi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">M.whilo</t>
+  </si>
+  <si>
     <t xml:space="preserve">I.reg1_o</t>
   </si>
   <si>
+    <t xml:space="preserve">EM.hilo_o</t>
+  </si>
+  <si>
     <t xml:space="preserve">I.reg1_addr_o</t>
   </si>
   <si>
+    <t xml:space="preserve">EM.cnt_o</t>
+  </si>
+  <si>
+    <t xml:space="preserve">E.stallreq</t>
+  </si>
+  <si>
     <t xml:space="preserve">I.reg2_o</t>
   </si>
   <si>
+    <t xml:space="preserve">DIV.result_o</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I.stallreq</t>
+  </si>
+  <si>
     <t xml:space="preserve">I.reg2_addr_o</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DIV.ready_o</t>
   </si>
   <si>
     <t xml:space="preserve">控制信号→</t>
@@ -4859,6 +4901,10 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="27" fillId="5" borderId="33" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="27" fillId="3" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -4876,10 +4922,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="18" fillId="5" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="27" fillId="5" borderId="33" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -5055,9 +5097,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>5694480</xdr:colOff>
+      <xdr:colOff>5694120</xdr:colOff>
       <xdr:row>59</xdr:row>
-      <xdr:rowOff>324000</xdr:rowOff>
+      <xdr:rowOff>323640</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -5071,7 +5113,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="930240" y="27431280"/>
-          <a:ext cx="8421840" cy="2082960"/>
+          <a:ext cx="8440200" cy="2082600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -5092,9 +5134,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>23</xdr:col>
-      <xdr:colOff>118080</xdr:colOff>
+      <xdr:colOff>117720</xdr:colOff>
       <xdr:row>54</xdr:row>
-      <xdr:rowOff>188640</xdr:rowOff>
+      <xdr:rowOff>188280</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -5107,8 +5149,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="21113640" y="22780800"/>
-          <a:ext cx="8903160" cy="4692960"/>
+          <a:off x="21247200" y="22780800"/>
+          <a:ext cx="8902800" cy="4692600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -5130,17 +5172,17 @@
   </sheetPr>
   <dimension ref="C2:V36"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="50" zoomScaleNormal="50" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="40" zoomScaleNormal="40" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C37" activeCellId="0" sqref="C37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="30"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.57085020242915"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.9595141700405"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="19.6032388663968"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="84.6234817813765"/>
-    <col collapsed="false" hidden="false" max="9" min="5" style="0" width="12.9595141700405"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.0688259109312"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="19.7085020242915"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="85.3724696356275"/>
+    <col collapsed="false" hidden="false" max="9" min="5" style="0" width="13.0688259109312"/>
     <col collapsed="false" hidden="false" max="21" min="10" style="0" width="10.7125506072875"/>
     <col collapsed="false" hidden="false" max="1025" min="22" style="0" width="8.57085020242915"/>
   </cols>
@@ -7135,39 +7177,39 @@
   </sheetPr>
   <dimension ref="B1:AQ46"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="V1" colorId="64" zoomScale="50" zoomScaleNormal="50" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="40" zoomScaleNormal="40" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="U26" activeCellId="0" sqref="U26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="24.95"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="76" width="10.7125506072875"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="76" width="12.9595141700405"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="76" width="17.4615384615385"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="76" width="17.1376518218624"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="76" width="18.2105263157895"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="76" width="17.4615384615385"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="76" width="12.9595141700405"/>
-    <col collapsed="false" hidden="false" max="10" min="9" style="76" width="18.6396761133603"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="76" width="24.7449392712551"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="76" width="15.5303643724696"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="76" width="17.1376518218624"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="76" width="20.3522267206478"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="76" width="15.5303643724696"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="76" width="17.1376518218624"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="76" width="24.7449392712551"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="76" width="13.0688259109312"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="76" width="17.5668016194332"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="76" width="17.246963562753"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="76" width="18.3157894736842"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="76" width="17.5668016194332"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="76" width="13.0688259109312"/>
+    <col collapsed="false" hidden="false" max="10" min="9" style="76" width="18.7449392712551"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="76" width="24.9595141700405"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="76" width="15.6396761133603"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="76" width="17.246963562753"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="76" width="20.4615384615385"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="76" width="15.6396761133603"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="76" width="17.246963562753"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="76" width="24.9595141700405"/>
     <col collapsed="false" hidden="false" max="18" min="18" style="76" width="13.7125506072874"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="76" width="17.1376518218624"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="76" width="21.9595141700405"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="76" width="15.5303643724696"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="76" width="17.246963562753"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="76" width="22.1740890688259"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="76" width="15.6396761133603"/>
     <col collapsed="false" hidden="false" max="22" min="22" style="76" width="10.7125506072875"/>
-    <col collapsed="false" hidden="false" max="23" min="23" style="76" width="21.9595141700405"/>
-    <col collapsed="false" hidden="false" max="24" min="24" style="76" width="12.3198380566802"/>
+    <col collapsed="false" hidden="false" max="23" min="23" style="76" width="22.1740890688259"/>
+    <col collapsed="false" hidden="false" max="24" min="24" style="76" width="12.4251012145749"/>
     <col collapsed="false" hidden="false" max="25" min="25" style="76" width="10.7125506072875"/>
-    <col collapsed="false" hidden="false" max="26" min="26" style="76" width="21.9595141700405"/>
-    <col collapsed="false" hidden="false" max="27" min="27" style="76" width="15.5303643724696"/>
+    <col collapsed="false" hidden="false" max="26" min="26" style="76" width="22.1740890688259"/>
+    <col collapsed="false" hidden="false" max="27" min="27" style="76" width="15.6396761133603"/>
     <col collapsed="false" hidden="false" max="28" min="28" style="76" width="10.7125506072875"/>
-    <col collapsed="false" hidden="false" max="29" min="29" style="76" width="23.0323886639676"/>
+    <col collapsed="false" hidden="false" max="29" min="29" style="76" width="23.1376518218623"/>
     <col collapsed="false" hidden="false" max="1025" min="30" style="76" width="10.7125506072875"/>
   </cols>
   <sheetData>
@@ -9637,17 +9679,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="B4:X27"/>
+  <dimension ref="A4:AA27"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="50" zoomScaleNormal="50" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D22" activeCellId="0" sqref="D22"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="M1" colorId="64" zoomScale="40" zoomScaleNormal="40" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="R25" activeCellId="0" sqref="R25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.57085020242915"/>
-    <col collapsed="false" hidden="false" max="24" min="2" style="0" width="20.995951417004"/>
-    <col collapsed="false" hidden="false" max="27" min="25" style="0" width="15.9595141700405"/>
+    <col collapsed="false" hidden="false" max="24" min="2" style="0" width="21.1012145748988"/>
+    <col collapsed="false" hidden="false" max="27" min="25" style="0" width="16.0688259109312"/>
     <col collapsed="false" hidden="false" max="1025" min="28" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -9690,270 +9732,317 @@
         <v>133</v>
       </c>
       <c r="X4" s="122"/>
+      <c r="Z4" s="122" t="s">
+        <v>136</v>
+      </c>
+      <c r="AA4" s="122"/>
     </row>
     <row r="5" customFormat="false" ht="21.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B5" s="124" t="s">
+      <c r="A5" s="124" t="s">
         <v>138</v>
       </c>
-      <c r="C5" s="125" t="s">
+      <c r="B5" s="125" t="s">
+        <v>138</v>
+      </c>
+      <c r="C5" s="126" t="s">
         <v>142</v>
       </c>
-      <c r="D5" s="126"/>
-      <c r="E5" s="124" t="s">
+      <c r="D5" s="127"/>
+      <c r="E5" s="125" t="s">
         <v>140</v>
       </c>
-      <c r="F5" s="125" t="s">
+      <c r="F5" s="126" t="s">
         <v>278</v>
       </c>
-      <c r="G5" s="126"/>
-      <c r="H5" s="124" t="s">
+      <c r="G5" s="127"/>
+      <c r="H5" s="125" t="s">
         <v>143</v>
       </c>
-      <c r="I5" s="125" t="s">
+      <c r="I5" s="126" t="s">
         <v>279</v>
       </c>
-      <c r="J5" s="126"/>
-      <c r="K5" s="124" t="s">
+      <c r="J5" s="127"/>
+      <c r="K5" s="125" t="s">
         <v>147</v>
       </c>
-      <c r="L5" s="125" t="s">
+      <c r="L5" s="126" t="s">
         <v>282</v>
       </c>
-      <c r="M5" s="126"/>
-      <c r="N5" s="124" t="s">
+      <c r="M5" s="127"/>
+      <c r="N5" s="125" t="s">
         <v>179</v>
       </c>
-      <c r="O5" s="125" t="s">
+      <c r="O5" s="126" t="s">
         <v>283</v>
       </c>
-      <c r="P5" s="126"/>
-      <c r="Q5" s="124" t="s">
+      <c r="P5" s="127"/>
+      <c r="Q5" s="125" t="s">
         <v>181</v>
       </c>
-      <c r="R5" s="125" t="s">
+      <c r="R5" s="126" t="s">
         <v>185</v>
       </c>
-      <c r="S5" s="126"/>
-      <c r="T5" s="124" t="s">
+      <c r="S5" s="127"/>
+      <c r="T5" s="125" t="s">
         <v>166</v>
       </c>
-      <c r="U5" s="125" t="s">
+      <c r="U5" s="126" t="s">
         <v>283</v>
       </c>
-      <c r="V5" s="126"/>
-      <c r="W5" s="127" t="s">
+      <c r="V5" s="127"/>
+      <c r="W5" s="128" t="s">
         <v>185</v>
       </c>
-      <c r="X5" s="128" t="s">
-        <v>284</v>
+      <c r="X5" s="129" t="s">
+        <v>314</v>
+      </c>
+      <c r="Y5" s="127"/>
+      <c r="Z5" s="128" t="s">
+        <v>190</v>
+      </c>
+      <c r="AA5" s="129" t="s">
+        <v>287</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="21.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B6" s="124" t="s">
+      <c r="A6" s="124" t="s">
         <v>151</v>
       </c>
-      <c r="C6" s="125" t="s">
+      <c r="B6" s="125" t="s">
+        <v>151</v>
+      </c>
+      <c r="C6" s="126" t="s">
         <v>289</v>
       </c>
       <c r="D6" s="123"/>
-      <c r="E6" s="124" t="s">
+      <c r="E6" s="125" t="s">
         <v>153</v>
       </c>
-      <c r="F6" s="125" t="s">
+      <c r="F6" s="126" t="s">
         <v>291</v>
       </c>
-      <c r="G6" s="126"/>
-      <c r="H6" s="124" t="s">
+      <c r="G6" s="127"/>
+      <c r="H6" s="125" t="s">
         <v>156</v>
       </c>
-      <c r="I6" s="125" t="s">
+      <c r="I6" s="126" t="s">
         <v>292</v>
       </c>
-      <c r="J6" s="126"/>
-      <c r="K6" s="124" t="s">
+      <c r="J6" s="127"/>
+      <c r="K6" s="125" t="s">
         <v>161</v>
       </c>
-      <c r="L6" s="125" t="s">
+      <c r="L6" s="126" t="s">
         <v>295</v>
       </c>
-      <c r="M6" s="126"/>
-      <c r="N6" s="124" t="s">
+      <c r="M6" s="127"/>
+      <c r="N6" s="125" t="s">
         <v>164</v>
       </c>
-      <c r="O6" s="125" t="s">
+      <c r="O6" s="126" t="s">
         <v>296</v>
       </c>
-      <c r="P6" s="126"/>
-      <c r="Q6" s="124" t="s">
+      <c r="P6" s="127"/>
+      <c r="Q6" s="125" t="s">
         <v>199</v>
       </c>
-      <c r="R6" s="125" t="s">
+      <c r="R6" s="126" t="s">
         <v>202</v>
       </c>
-      <c r="S6" s="126"/>
-      <c r="T6" s="124" t="s">
+      <c r="S6" s="127"/>
+      <c r="T6" s="125" t="s">
         <v>183</v>
       </c>
-      <c r="U6" s="125" t="s">
+      <c r="U6" s="126" t="s">
         <v>296</v>
       </c>
-      <c r="V6" s="126"/>
-      <c r="W6" s="127" t="s">
+      <c r="V6" s="127"/>
+      <c r="W6" s="128" t="s">
         <v>202</v>
       </c>
-      <c r="X6" s="128" t="s">
-        <v>297</v>
+      <c r="X6" s="129" t="s">
+        <v>320</v>
+      </c>
+      <c r="Y6" s="127"/>
+      <c r="Z6" s="128" t="s">
+        <v>205</v>
+      </c>
+      <c r="AA6" s="129" t="s">
+        <v>299</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="21.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B7" s="123"/>
+      <c r="A7" s="124" t="s">
+        <v>345</v>
+      </c>
+      <c r="B7" s="125" t="s">
+        <v>171</v>
+      </c>
       <c r="C7" s="123"/>
-      <c r="D7" s="129" t="s">
+      <c r="D7" s="124" t="s">
         <v>138</v>
       </c>
-      <c r="E7" s="124" t="s">
+      <c r="E7" s="125" t="s">
         <v>138</v>
       </c>
       <c r="F7" s="123"/>
-      <c r="G7" s="129" t="s">
-        <v>345</v>
-      </c>
-      <c r="H7" s="124" t="s">
+      <c r="G7" s="124" t="s">
+        <v>346</v>
+      </c>
+      <c r="H7" s="125" t="s">
         <v>173</v>
       </c>
-      <c r="I7" s="125" t="s">
+      <c r="I7" s="126" t="s">
         <v>301</v>
       </c>
-      <c r="J7" s="126"/>
-      <c r="K7" s="124" t="s">
+      <c r="J7" s="127"/>
+      <c r="K7" s="125" t="s">
         <v>177</v>
       </c>
-      <c r="L7" s="125" t="s">
+      <c r="L7" s="126" t="s">
         <v>303</v>
       </c>
-      <c r="M7" s="126"/>
-      <c r="N7" s="124" t="s">
+      <c r="M7" s="127"/>
+      <c r="N7" s="125" t="s">
         <v>198</v>
       </c>
-      <c r="O7" s="125" t="s">
+      <c r="O7" s="126" t="s">
         <v>304</v>
       </c>
-      <c r="P7" s="126"/>
-      <c r="Q7" s="124" t="s">
+      <c r="P7" s="127"/>
+      <c r="Q7" s="125" t="s">
         <v>212</v>
       </c>
-      <c r="R7" s="125" t="s">
+      <c r="R7" s="126" t="s">
         <v>305</v>
       </c>
-      <c r="S7" s="126"/>
-      <c r="T7" s="124" t="s">
+      <c r="S7" s="127"/>
+      <c r="T7" s="125" t="s">
         <v>200</v>
       </c>
-      <c r="U7" s="125" t="s">
+      <c r="U7" s="126" t="s">
         <v>304</v>
       </c>
-      <c r="V7" s="126"/>
-      <c r="W7" s="127" t="s">
-        <v>215</v>
-      </c>
-      <c r="X7" s="128" t="s">
-        <v>306</v>
+      <c r="V7" s="127"/>
+      <c r="W7" s="128" t="s">
+        <v>305</v>
+      </c>
+      <c r="X7" s="129" t="s">
+        <v>325</v>
+      </c>
+      <c r="Y7" s="127"/>
+      <c r="Z7" s="128" t="s">
+        <v>218</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="21.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B8" s="123"/>
       <c r="C8" s="123"/>
-      <c r="D8" s="129" t="s">
+      <c r="D8" s="124" t="s">
         <v>151</v>
       </c>
-      <c r="E8" s="124" t="s">
+      <c r="E8" s="125" t="s">
         <v>151</v>
       </c>
       <c r="F8" s="123"/>
-      <c r="G8" s="129" t="s">
-        <v>346</v>
-      </c>
-      <c r="H8" s="124" t="s">
+      <c r="G8" s="124" t="s">
+        <v>347</v>
+      </c>
+      <c r="H8" s="125" t="s">
         <v>192</v>
       </c>
-      <c r="I8" s="125" t="s">
+      <c r="I8" s="126" t="s">
         <v>307</v>
       </c>
-      <c r="J8" s="126"/>
-      <c r="K8" s="124" t="s">
+      <c r="J8" s="127"/>
+      <c r="K8" s="125" t="s">
         <v>196</v>
       </c>
-      <c r="L8" s="125" t="s">
+      <c r="L8" s="126" t="s">
         <v>309</v>
       </c>
-      <c r="M8" s="126"/>
-      <c r="N8" s="124" t="s">
+      <c r="M8" s="127"/>
+      <c r="N8" s="125" t="s">
         <v>211</v>
       </c>
-      <c r="O8" s="123"/>
-      <c r="P8" s="129" t="s">
-        <v>138</v>
-      </c>
-      <c r="Q8" s="124" t="s">
-        <v>138</v>
-      </c>
-      <c r="R8" s="123"/>
-      <c r="S8" s="129" t="s">
-        <v>138</v>
-      </c>
-      <c r="T8" s="124" t="s">
-        <v>138</v>
-      </c>
-      <c r="U8" s="123"/>
-      <c r="V8" s="129" t="s">
-        <v>138</v>
-      </c>
-      <c r="W8" s="127" t="s">
-        <v>138</v>
+      <c r="O8" s="126" t="s">
+        <v>287</v>
+      </c>
+      <c r="P8" s="127"/>
+      <c r="Q8" s="125" t="s">
+        <v>252</v>
+      </c>
+      <c r="R8" s="126" t="s">
+        <v>246</v>
+      </c>
+      <c r="S8" s="127"/>
+      <c r="T8" s="125" t="s">
+        <v>205</v>
+      </c>
+      <c r="U8" s="126" t="s">
+        <v>287</v>
+      </c>
+      <c r="V8" s="127"/>
+      <c r="W8" s="128" t="s">
+        <v>246</v>
+      </c>
+      <c r="X8" s="129" t="s">
+        <v>284</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="21.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B9" s="123"/>
       <c r="C9" s="123"/>
-      <c r="D9" s="123"/>
-      <c r="E9" s="123"/>
+      <c r="D9" s="124" t="s">
+        <v>345</v>
+      </c>
+      <c r="E9" s="125" t="s">
+        <v>171</v>
+      </c>
       <c r="F9" s="123"/>
-      <c r="G9" s="129" t="s">
-        <v>347</v>
-      </c>
-      <c r="H9" s="124" t="s">
+      <c r="G9" s="124" t="s">
+        <v>348</v>
+      </c>
+      <c r="H9" s="125" t="s">
         <v>207</v>
       </c>
-      <c r="I9" s="125" t="s">
+      <c r="I9" s="126" t="s">
         <v>296</v>
       </c>
-      <c r="J9" s="126"/>
-      <c r="K9" s="124" t="s">
+      <c r="J9" s="127"/>
+      <c r="K9" s="125" t="s">
         <v>210</v>
       </c>
-      <c r="L9" s="125" t="s">
+      <c r="L9" s="126" t="s">
         <v>199</v>
       </c>
-      <c r="M9" s="126"/>
-      <c r="N9" s="124" t="s">
+      <c r="M9" s="127"/>
+      <c r="N9" s="125" t="s">
         <v>183</v>
       </c>
-      <c r="O9" s="123"/>
-      <c r="P9" s="129" t="s">
-        <v>151</v>
-      </c>
-      <c r="Q9" s="124" t="s">
-        <v>151</v>
-      </c>
-      <c r="R9" s="123"/>
-      <c r="S9" s="123"/>
-      <c r="T9" s="123"/>
-      <c r="U9" s="123"/>
-      <c r="V9" s="129" t="s">
-        <v>151</v>
-      </c>
-      <c r="W9" s="127" t="s">
-        <v>151</v>
+      <c r="O9" s="126" t="s">
+        <v>299</v>
+      </c>
+      <c r="P9" s="127"/>
+      <c r="Q9" s="125" t="s">
+        <v>260</v>
+      </c>
+      <c r="R9" s="126" t="s">
+        <v>254</v>
+      </c>
+      <c r="S9" s="127"/>
+      <c r="T9" s="125" t="s">
+        <v>218</v>
+      </c>
+      <c r="U9" s="126" t="s">
+        <v>299</v>
+      </c>
+      <c r="V9" s="127"/>
+      <c r="W9" s="128" t="s">
+        <v>254</v>
+      </c>
+      <c r="X9" s="129" t="s">
+        <v>297</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="21.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -9962,33 +10051,50 @@
       <c r="D10" s="123"/>
       <c r="E10" s="123"/>
       <c r="F10" s="123"/>
-      <c r="G10" s="129" t="s">
-        <v>348</v>
-      </c>
-      <c r="H10" s="124" t="s">
+      <c r="G10" s="124" t="s">
+        <v>349</v>
+      </c>
+      <c r="H10" s="125" t="s">
         <v>220</v>
       </c>
-      <c r="I10" s="125" t="s">
+      <c r="I10" s="126" t="s">
         <v>304</v>
       </c>
-      <c r="J10" s="126"/>
-      <c r="K10" s="124" t="s">
+      <c r="J10" s="127"/>
+      <c r="K10" s="125" t="s">
         <v>224</v>
       </c>
-      <c r="L10" s="125" t="s">
+      <c r="L10" s="126" t="s">
         <v>212</v>
       </c>
-      <c r="M10" s="126"/>
-      <c r="N10" s="124" t="s">
+      <c r="M10" s="127"/>
+      <c r="N10" s="125" t="s">
         <v>200</v>
       </c>
-      <c r="O10" s="123"/>
-      <c r="P10" s="123"/>
-      <c r="Q10" s="123"/>
-      <c r="R10" s="123"/>
-      <c r="S10" s="123"/>
-      <c r="T10" s="123"/>
-      <c r="U10" s="123"/>
+      <c r="O10" s="126" t="s">
+        <v>312</v>
+      </c>
+      <c r="P10" s="127"/>
+      <c r="Q10" s="125" t="s">
+        <v>244</v>
+      </c>
+      <c r="R10" s="126" t="s">
+        <v>237</v>
+      </c>
+      <c r="S10" s="127"/>
+      <c r="T10" s="125" t="s">
+        <v>213</v>
+      </c>
+      <c r="U10" s="126" t="s">
+        <v>312</v>
+      </c>
+      <c r="V10" s="127"/>
+      <c r="W10" s="128" t="s">
+        <v>237</v>
+      </c>
+      <c r="X10" s="129" t="s">
+        <v>306</v>
+      </c>
     </row>
     <row r="11" customFormat="false" ht="21.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B11" s="123"/>
@@ -9996,35 +10102,55 @@
       <c r="D11" s="123"/>
       <c r="E11" s="123"/>
       <c r="F11" s="123"/>
-      <c r="G11" s="129" t="s">
-        <v>349</v>
-      </c>
-      <c r="H11" s="124" t="s">
+      <c r="G11" s="124" t="s">
+        <v>350</v>
+      </c>
+      <c r="H11" s="125" t="s">
         <v>230</v>
       </c>
-      <c r="I11" s="125" t="s">
+      <c r="I11" s="126" t="s">
         <v>327</v>
       </c>
-      <c r="J11" s="129" t="s">
+      <c r="J11" s="124" t="s">
         <v>138</v>
       </c>
-      <c r="K11" s="124" t="s">
+      <c r="K11" s="125" t="s">
         <v>138</v>
       </c>
       <c r="L11" s="123"/>
-      <c r="M11" s="129" t="s">
+      <c r="M11" s="124" t="s">
+        <v>351</v>
+      </c>
+      <c r="N11" s="125" t="s">
+        <v>205</v>
+      </c>
+      <c r="O11" s="126" t="s">
+        <v>334</v>
+      </c>
+      <c r="P11" s="127"/>
+      <c r="Q11" s="125" t="s">
+        <v>225</v>
+      </c>
+      <c r="R11" s="123"/>
+      <c r="S11" s="124" t="s">
         <v>138</v>
       </c>
-      <c r="N11" s="124" t="s">
+      <c r="T11" s="125" t="s">
         <v>138</v>
       </c>
-      <c r="O11" s="123"/>
-      <c r="P11" s="123"/>
-      <c r="Q11" s="123"/>
-      <c r="R11" s="123"/>
-      <c r="S11" s="123"/>
-      <c r="T11" s="123"/>
       <c r="U11" s="123"/>
+      <c r="V11" s="124" t="s">
+        <v>138</v>
+      </c>
+      <c r="W11" s="128" t="s">
+        <v>138</v>
+      </c>
+      <c r="Y11" s="124" t="s">
+        <v>138</v>
+      </c>
+      <c r="Z11" s="128" t="s">
+        <v>138</v>
+      </c>
     </row>
     <row r="12" customFormat="false" ht="21.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B12" s="123"/>
@@ -10032,31 +10158,53 @@
       <c r="D12" s="123"/>
       <c r="E12" s="123"/>
       <c r="F12" s="123"/>
-      <c r="G12" s="129" t="s">
-        <v>350</v>
-      </c>
-      <c r="H12" s="124" t="s">
+      <c r="G12" s="124" t="s">
+        <v>352</v>
+      </c>
+      <c r="H12" s="125" t="s">
         <v>240</v>
       </c>
-      <c r="I12" s="125" t="s">
+      <c r="I12" s="126" t="s">
         <v>332</v>
       </c>
-      <c r="J12" s="129" t="s">
+      <c r="J12" s="124" t="s">
         <v>151</v>
       </c>
-      <c r="K12" s="124" t="s">
+      <c r="K12" s="125" t="s">
         <v>151</v>
       </c>
       <c r="L12" s="123"/>
-      <c r="M12" s="123"/>
-      <c r="N12" s="123"/>
-      <c r="O12" s="123"/>
-      <c r="P12" s="123"/>
-      <c r="Q12" s="123"/>
-      <c r="R12" s="123"/>
+      <c r="M12" s="124" t="s">
+        <v>353</v>
+      </c>
+      <c r="N12" s="125" t="s">
+        <v>218</v>
+      </c>
+      <c r="O12" s="126" t="s">
+        <v>317</v>
+      </c>
+      <c r="P12" s="127"/>
+      <c r="Q12" s="125" t="s">
+        <v>234</v>
+      </c>
+      <c r="R12" s="126" t="s">
+        <v>311</v>
+      </c>
       <c r="S12" s="123"/>
       <c r="T12" s="123"/>
       <c r="U12" s="123"/>
+      <c r="V12" s="124" t="s">
+        <v>151</v>
+      </c>
+      <c r="W12" s="128" t="s">
+        <v>151</v>
+      </c>
+      <c r="Y12" s="124" t="s">
+        <v>151</v>
+      </c>
+      <c r="Z12" s="128" t="s">
+        <v>151</v>
+      </c>
     </row>
     <row r="13" customFormat="false" ht="21.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B13" s="123"/>
@@ -10064,27 +10212,47 @@
       <c r="D13" s="123"/>
       <c r="E13" s="123"/>
       <c r="F13" s="123"/>
-      <c r="G13" s="129" t="s">
-        <v>351</v>
-      </c>
-      <c r="H13" s="124" t="s">
+      <c r="G13" s="124" t="s">
+        <v>354</v>
+      </c>
+      <c r="H13" s="125" t="s">
         <v>248</v>
       </c>
-      <c r="I13" s="125" t="s">
+      <c r="I13" s="126" t="s">
         <v>336</v>
       </c>
-      <c r="J13" s="123"/>
-      <c r="K13" s="123"/>
+      <c r="J13" s="124" t="s">
+        <v>345</v>
+      </c>
+      <c r="K13" s="125" t="s">
+        <v>171</v>
+      </c>
       <c r="L13" s="123"/>
-      <c r="M13" s="123"/>
-      <c r="N13" s="123"/>
+      <c r="M13" s="124" t="s">
+        <v>355</v>
+      </c>
+      <c r="N13" s="125" t="s">
+        <v>273</v>
+      </c>
       <c r="O13" s="123"/>
-      <c r="P13" s="123"/>
-      <c r="Q13" s="123"/>
-      <c r="R13" s="123"/>
+      <c r="P13" s="124" t="s">
+        <v>138</v>
+      </c>
+      <c r="Q13" s="125" t="s">
+        <v>138</v>
+      </c>
+      <c r="R13" s="126" t="s">
+        <v>317</v>
+      </c>
       <c r="S13" s="123"/>
       <c r="T13" s="123"/>
       <c r="U13" s="123"/>
+      <c r="V13" s="124" t="s">
+        <v>356</v>
+      </c>
+      <c r="W13" s="125" t="s">
+        <v>171</v>
+      </c>
     </row>
     <row r="14" customFormat="false" ht="21.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B14" s="123"/>
@@ -10092,23 +10260,31 @@
       <c r="D14" s="123"/>
       <c r="E14" s="123"/>
       <c r="F14" s="123"/>
-      <c r="G14" s="129" t="s">
-        <v>352</v>
-      </c>
-      <c r="H14" s="124" t="s">
+      <c r="G14" s="124" t="s">
+        <v>357</v>
+      </c>
+      <c r="H14" s="125" t="s">
         <v>256</v>
       </c>
-      <c r="I14" s="125" t="s">
+      <c r="I14" s="126" t="s">
         <v>338</v>
       </c>
       <c r="J14" s="123"/>
       <c r="K14" s="123"/>
       <c r="L14" s="123"/>
-      <c r="M14" s="123"/>
-      <c r="N14" s="123"/>
+      <c r="M14" s="124" t="s">
+        <v>355</v>
+      </c>
+      <c r="N14" s="125" t="s">
+        <v>275</v>
+      </c>
       <c r="O14" s="123"/>
-      <c r="P14" s="123"/>
-      <c r="Q14" s="123"/>
+      <c r="P14" s="124" t="s">
+        <v>151</v>
+      </c>
+      <c r="Q14" s="125" t="s">
+        <v>151</v>
+      </c>
       <c r="R14" s="123"/>
       <c r="S14" s="123"/>
       <c r="T14" s="123"/>
@@ -10120,24 +10296,32 @@
       <c r="D15" s="123"/>
       <c r="E15" s="123"/>
       <c r="F15" s="123"/>
-      <c r="G15" s="129" t="s">
+      <c r="G15" s="124" t="s">
         <v>138</v>
       </c>
-      <c r="H15" s="124" t="s">
+      <c r="H15" s="125" t="s">
         <v>138</v>
       </c>
-      <c r="I15" s="123"/>
+      <c r="I15" s="126" t="s">
+        <v>341</v>
+      </c>
       <c r="J15" s="123"/>
       <c r="K15" s="123"/>
       <c r="L15" s="123"/>
-      <c r="M15" s="123"/>
-      <c r="N15" s="123"/>
+      <c r="M15" s="124" t="s">
+        <v>358</v>
+      </c>
+      <c r="N15" s="125" t="s">
+        <v>314</v>
+      </c>
       <c r="O15" s="123"/>
-      <c r="P15" s="123"/>
-      <c r="Q15" s="123"/>
+      <c r="P15" s="124" t="s">
+        <v>345</v>
+      </c>
+      <c r="Q15" s="125" t="s">
+        <v>171</v>
+      </c>
       <c r="R15" s="123"/>
-      <c r="S15" s="123"/>
-      <c r="T15" s="123"/>
       <c r="U15" s="123"/>
     </row>
     <row r="16" customFormat="false" ht="21.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -10152,9 +10336,15 @@
       <c r="J16" s="123"/>
       <c r="K16" s="123"/>
       <c r="L16" s="123"/>
-      <c r="M16" s="123"/>
-      <c r="N16" s="123"/>
-      <c r="O16" s="123"/>
+      <c r="M16" s="124" t="s">
+        <v>359</v>
+      </c>
+      <c r="N16" s="125" t="s">
+        <v>267</v>
+      </c>
+      <c r="O16" s="126" t="s">
+        <v>341</v>
+      </c>
       <c r="P16" s="123"/>
       <c r="Q16" s="123"/>
       <c r="R16" s="123"/>
@@ -10174,8 +10364,12 @@
       <c r="J17" s="123"/>
       <c r="K17" s="123"/>
       <c r="L17" s="123"/>
-      <c r="M17" s="123"/>
-      <c r="N17" s="123"/>
+      <c r="M17" s="124" t="s">
+        <v>359</v>
+      </c>
+      <c r="N17" s="125" t="s">
+        <v>269</v>
+      </c>
       <c r="O17" s="123"/>
       <c r="P17" s="123"/>
       <c r="Q17" s="123"/>
@@ -10198,8 +10392,12 @@
       <c r="J18" s="123"/>
       <c r="K18" s="123"/>
       <c r="L18" s="123"/>
-      <c r="M18" s="123"/>
-      <c r="N18" s="123"/>
+      <c r="M18" s="124" t="s">
+        <v>360</v>
+      </c>
+      <c r="N18" s="125" t="s">
+        <v>265</v>
+      </c>
       <c r="O18" s="123"/>
       <c r="P18" s="123"/>
       <c r="Q18" s="123"/>
@@ -10214,20 +10412,24 @@
       <c r="D19" s="123"/>
       <c r="E19" s="123"/>
       <c r="F19" s="123"/>
-      <c r="G19" s="129" t="s">
-        <v>353</v>
-      </c>
-      <c r="H19" s="124" t="s">
+      <c r="G19" s="124" t="s">
+        <v>361</v>
+      </c>
+      <c r="H19" s="125" t="s">
         <v>145</v>
       </c>
-      <c r="I19" s="125" t="s">
+      <c r="I19" s="126" t="s">
         <v>280</v>
       </c>
       <c r="J19" s="123"/>
       <c r="K19" s="123"/>
       <c r="L19" s="123"/>
-      <c r="M19" s="123"/>
-      <c r="N19" s="123"/>
+      <c r="M19" s="124" t="s">
+        <v>362</v>
+      </c>
+      <c r="N19" s="125" t="s">
+        <v>258</v>
+      </c>
       <c r="O19" s="123"/>
       <c r="P19" s="123"/>
       <c r="Q19" s="123"/>
@@ -10235,6 +10437,10 @@
       <c r="S19" s="123"/>
       <c r="T19" s="123"/>
       <c r="U19" s="123"/>
+      <c r="Z19" s="122" t="s">
+        <v>135</v>
+      </c>
+      <c r="AA19" s="122"/>
     </row>
     <row r="20" customFormat="false" ht="21.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B20" s="123"/>
@@ -10242,20 +10448,24 @@
       <c r="D20" s="123"/>
       <c r="E20" s="123"/>
       <c r="F20" s="123"/>
-      <c r="G20" s="129" t="s">
-        <v>354</v>
-      </c>
-      <c r="H20" s="124" t="s">
+      <c r="G20" s="124" t="s">
+        <v>363</v>
+      </c>
+      <c r="H20" s="125" t="s">
         <v>158</v>
       </c>
-      <c r="I20" s="125" t="s">
+      <c r="I20" s="126" t="s">
         <v>293</v>
       </c>
       <c r="J20" s="123"/>
       <c r="K20" s="123"/>
       <c r="L20" s="123"/>
-      <c r="M20" s="123"/>
-      <c r="N20" s="123"/>
+      <c r="M20" s="124" t="s">
+        <v>364</v>
+      </c>
+      <c r="N20" s="125" t="s">
+        <v>234</v>
+      </c>
       <c r="O20" s="123"/>
       <c r="P20" s="123"/>
       <c r="Q20" s="123"/>
@@ -10263,6 +10473,15 @@
       <c r="S20" s="123"/>
       <c r="T20" s="123"/>
       <c r="U20" s="123"/>
+      <c r="Y20" s="124" t="s">
+        <v>365</v>
+      </c>
+      <c r="Z20" s="128" t="s">
+        <v>188</v>
+      </c>
+      <c r="AA20" s="129" t="s">
+        <v>171</v>
+      </c>
     </row>
     <row r="21" customFormat="false" ht="21.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B21" s="123"/>
@@ -10270,18 +10489,22 @@
       <c r="D21" s="123"/>
       <c r="E21" s="123"/>
       <c r="F21" s="123"/>
-      <c r="G21" s="129" t="s">
-        <v>355</v>
-      </c>
-      <c r="H21" s="124" t="s">
+      <c r="G21" s="124" t="s">
+        <v>366</v>
+      </c>
+      <c r="H21" s="125" t="s">
         <v>175</v>
       </c>
       <c r="I21" s="123"/>
       <c r="J21" s="123"/>
       <c r="K21" s="123"/>
       <c r="L21" s="123"/>
-      <c r="M21" s="123"/>
-      <c r="N21" s="123"/>
+      <c r="M21" s="124" t="s">
+        <v>367</v>
+      </c>
+      <c r="N21" s="125" t="s">
+        <v>242</v>
+      </c>
       <c r="O21" s="123"/>
       <c r="P21" s="123"/>
       <c r="Q21" s="123"/>
@@ -10289,6 +10512,12 @@
       <c r="S21" s="123"/>
       <c r="T21" s="123"/>
       <c r="U21" s="123"/>
+      <c r="Y21" s="124" t="s">
+        <v>368</v>
+      </c>
+      <c r="Z21" s="128" t="s">
+        <v>169</v>
+      </c>
     </row>
     <row r="22" customFormat="false" ht="21.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B22" s="123"/>
@@ -10296,25 +10525,33 @@
       <c r="D22" s="123"/>
       <c r="E22" s="123"/>
       <c r="F22" s="123"/>
-      <c r="G22" s="129" t="s">
-        <v>356</v>
-      </c>
-      <c r="H22" s="124" t="s">
+      <c r="G22" s="124" t="s">
+        <v>369</v>
+      </c>
+      <c r="H22" s="125" t="s">
         <v>194</v>
       </c>
       <c r="I22" s="123"/>
       <c r="J22" s="123"/>
       <c r="K22" s="123"/>
       <c r="L22" s="123"/>
-      <c r="M22" s="123"/>
-      <c r="N22" s="123"/>
+      <c r="M22" s="124" t="s">
+        <v>370</v>
+      </c>
+      <c r="N22" s="125" t="s">
+        <v>250</v>
+      </c>
       <c r="O22" s="123"/>
-      <c r="P22" s="123"/>
-      <c r="Q22" s="123"/>
       <c r="R22" s="123"/>
       <c r="S22" s="123"/>
       <c r="T22" s="123"/>
       <c r="U22" s="123"/>
+      <c r="Y22" s="124" t="s">
+        <v>151</v>
+      </c>
+      <c r="Z22" s="128" t="s">
+        <v>138</v>
+      </c>
     </row>
     <row r="23" customFormat="false" ht="21.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B23" s="123"/>
@@ -10322,21 +10559,23 @@
       <c r="D23" s="123"/>
       <c r="E23" s="123"/>
       <c r="F23" s="123"/>
-      <c r="G23" s="129" t="s">
-        <v>350</v>
-      </c>
-      <c r="H23" s="124" t="s">
+      <c r="G23" s="124" t="s">
+        <v>352</v>
+      </c>
+      <c r="H23" s="125" t="s">
         <v>190</v>
       </c>
       <c r="I23" s="123"/>
       <c r="J23" s="123"/>
       <c r="K23" s="123"/>
       <c r="L23" s="123"/>
-      <c r="M23" s="123"/>
-      <c r="N23" s="123"/>
+      <c r="M23" s="124" t="s">
+        <v>138</v>
+      </c>
+      <c r="N23" s="125" t="s">
+        <v>138</v>
+      </c>
       <c r="O23" s="123"/>
-      <c r="P23" s="123"/>
-      <c r="Q23" s="123"/>
       <c r="R23" s="123"/>
       <c r="S23" s="123"/>
       <c r="T23" s="123"/>
@@ -10348,21 +10587,17 @@
       <c r="D24" s="123"/>
       <c r="E24" s="123"/>
       <c r="F24" s="123"/>
-      <c r="G24" s="129" t="s">
-        <v>351</v>
-      </c>
-      <c r="H24" s="124" t="s">
+      <c r="G24" s="124" t="s">
+        <v>354</v>
+      </c>
+      <c r="H24" s="125" t="s">
         <v>222</v>
       </c>
       <c r="I24" s="123"/>
       <c r="J24" s="123"/>
       <c r="K24" s="123"/>
       <c r="L24" s="123"/>
-      <c r="M24" s="123"/>
-      <c r="N24" s="123"/>
       <c r="O24" s="123"/>
-      <c r="P24" s="123"/>
-      <c r="Q24" s="123"/>
       <c r="R24" s="123"/>
       <c r="S24" s="123"/>
       <c r="T24" s="123"/>
@@ -10374,10 +10609,10 @@
       <c r="D25" s="123"/>
       <c r="E25" s="123"/>
       <c r="F25" s="123"/>
-      <c r="G25" s="129" t="s">
-        <v>352</v>
-      </c>
-      <c r="H25" s="124" t="s">
+      <c r="G25" s="124" t="s">
+        <v>357</v>
+      </c>
+      <c r="H25" s="125" t="s">
         <v>232</v>
       </c>
       <c r="I25" s="123"/>
@@ -10400,10 +10635,10 @@
       <c r="D26" s="123"/>
       <c r="E26" s="123"/>
       <c r="F26" s="123"/>
-      <c r="G26" s="129" t="s">
+      <c r="G26" s="124" t="s">
         <v>138</v>
       </c>
-      <c r="H26" s="124" t="s">
+      <c r="H26" s="125" t="s">
         <v>138</v>
       </c>
       <c r="I26" s="123"/>
@@ -10426,10 +10661,10 @@
       <c r="D27" s="123"/>
       <c r="E27" s="123"/>
       <c r="F27" s="123"/>
-      <c r="G27" s="129" t="s">
+      <c r="G27" s="124" t="s">
         <v>151</v>
       </c>
-      <c r="H27" s="124" t="s">
+      <c r="H27" s="125" t="s">
         <v>151</v>
       </c>
       <c r="I27" s="123"/>
@@ -10447,7 +10682,7 @@
       <c r="U27" s="123"/>
     </row>
   </sheetData>
-  <mergeCells count="9">
+  <mergeCells count="11">
     <mergeCell ref="B4:C4"/>
     <mergeCell ref="E4:F4"/>
     <mergeCell ref="H4:I4"/>
@@ -10456,7 +10691,9 @@
     <mergeCell ref="Q4:R4"/>
     <mergeCell ref="T4:U4"/>
     <mergeCell ref="W4:X4"/>
+    <mergeCell ref="Z4:AA4"/>
     <mergeCell ref="H18:I18"/>
+    <mergeCell ref="Z19:AA19"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -10475,64 +10712,64 @@
   </sheetPr>
   <dimension ref="B2:Q23"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="50" zoomScaleNormal="50" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="40" zoomScaleNormal="40" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="L53" activeCellId="0" sqref="L53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.57085020242915"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="12.9595141700405"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="46.8097165991903"/>
-    <col collapsed="false" hidden="false" max="17" min="5" style="0" width="12.9595141700405"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="13.0688259109312"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="47.1336032388664"/>
+    <col collapsed="false" hidden="false" max="17" min="5" style="0" width="13.0688259109312"/>
     <col collapsed="false" hidden="false" max="1025" min="18" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="3" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B3" s="1" t="s">
-        <v>357</v>
+        <v>371</v>
       </c>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
       <c r="E3" s="131" t="s">
-        <v>358</v>
+        <v>372</v>
       </c>
       <c r="F3" s="132" t="s">
-        <v>359</v>
+        <v>373</v>
       </c>
       <c r="G3" s="132" t="s">
-        <v>360</v>
+        <v>374</v>
       </c>
       <c r="H3" s="132" t="s">
-        <v>361</v>
+        <v>375</v>
       </c>
       <c r="I3" s="132" t="s">
-        <v>362</v>
+        <v>376</v>
       </c>
       <c r="J3" s="132" t="s">
-        <v>363</v>
+        <v>377</v>
       </c>
       <c r="K3" s="132" t="s">
-        <v>364</v>
+        <v>378</v>
       </c>
       <c r="L3" s="132" t="s">
-        <v>365</v>
+        <v>379</v>
       </c>
       <c r="M3" s="132" t="s">
-        <v>366</v>
+        <v>380</v>
       </c>
       <c r="N3" s="132" t="s">
-        <v>367</v>
+        <v>381</v>
       </c>
       <c r="O3" s="132" t="s">
-        <v>368</v>
+        <v>382</v>
       </c>
       <c r="P3" s="132" t="s">
-        <v>369</v>
+        <v>383</v>
       </c>
       <c r="Q3" s="133" t="s">
-        <v>370</v>
+        <v>384</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -10543,7 +10780,7 @@
         <v>71</v>
       </c>
       <c r="D4" s="136" t="s">
-        <v>371</v>
+        <v>385</v>
       </c>
       <c r="E4" s="137"/>
       <c r="F4" s="138" t="n">
@@ -10585,7 +10822,7 @@
         <v>80</v>
       </c>
       <c r="D5" s="22" t="s">
-        <v>372</v>
+        <v>386</v>
       </c>
       <c r="E5" s="141"/>
       <c r="F5" s="142" t="n">
@@ -10624,10 +10861,10 @@
     <row r="6" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B6" s="134"/>
       <c r="C6" s="144" t="s">
-        <v>373</v>
+        <v>387</v>
       </c>
       <c r="D6" s="12" t="s">
-        <v>374</v>
+        <v>388</v>
       </c>
       <c r="E6" s="145"/>
       <c r="F6" s="146" t="n">
@@ -10666,10 +10903,10 @@
     <row r="7" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B7" s="134"/>
       <c r="C7" s="144" t="s">
-        <v>375</v>
+        <v>389</v>
       </c>
       <c r="D7" s="12" t="s">
-        <v>376</v>
+        <v>390</v>
       </c>
       <c r="E7" s="145" t="n">
         <v>1</v>
@@ -10707,7 +10944,7 @@
         <v>16</v>
       </c>
       <c r="D8" s="22" t="s">
-        <v>377</v>
+        <v>391</v>
       </c>
       <c r="E8" s="141"/>
       <c r="F8" s="142" t="n">
@@ -10749,7 +10986,7 @@
         <v>44</v>
       </c>
       <c r="D9" s="12" t="s">
-        <v>378</v>
+        <v>392</v>
       </c>
       <c r="E9" s="145"/>
       <c r="F9" s="146" t="n">
@@ -10784,10 +11021,10 @@
     <row r="10" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B10" s="134"/>
       <c r="C10" s="144" t="s">
-        <v>379</v>
+        <v>393</v>
       </c>
       <c r="D10" s="12" t="s">
-        <v>380</v>
+        <v>394</v>
       </c>
       <c r="E10" s="145"/>
       <c r="F10" s="146"/>
@@ -10816,10 +11053,10 @@
     <row r="11" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B11" s="134"/>
       <c r="C11" s="140" t="s">
-        <v>381</v>
+        <v>395</v>
       </c>
       <c r="D11" s="22" t="s">
-        <v>382</v>
+        <v>396</v>
       </c>
       <c r="E11" s="141"/>
       <c r="F11" s="142" t="n">
@@ -10848,10 +11085,10 @@
     <row r="12" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B12" s="134"/>
       <c r="C12" s="144" t="s">
-        <v>383</v>
+        <v>397</v>
       </c>
       <c r="D12" s="12" t="s">
-        <v>384</v>
+        <v>398</v>
       </c>
       <c r="E12" s="145"/>
       <c r="F12" s="146"/>
@@ -10874,7 +11111,7 @@
     <row r="13" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B13" s="134"/>
       <c r="C13" s="144" t="s">
-        <v>385</v>
+        <v>399</v>
       </c>
       <c r="D13" s="12"/>
       <c r="E13" s="145"/>

</xml_diff>